<commit_message>
Many updates from Joel Tellinguisen comments.
</commit_message>
<xml_diff>
--- a/worksheets/ITC Worksheet for bovine CAII-CBS.xlsx
+++ b/worksheets/ITC Worksheet for bovine CAII-CBS.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="114">
   <si>
     <t>Notes</t>
   </si>
@@ -232,6 +232,9 @@
     <t>(need min 350 uL for VP-ITC)</t>
   </si>
   <si>
+    <t>assumes same pipette is used for stock solution and buffer</t>
+  </si>
+  <si>
     <t>titrant concentration</t>
   </si>
   <si>
@@ -253,7 +256,7 @@
     <t>Sigma-Aldrich C2522-25mg</t>
   </si>
   <si>
-    <t>molar extinction coefficient</t>
+    <t>molar absorptivity</t>
   </si>
   <si>
     <t>M-1 cm-1</t>
@@ -470,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
@@ -555,6 +558,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="8" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment wrapText="1"/>
     </xf>
@@ -585,6 +591,9 @@
     <xf borderId="0" fillId="4" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
@@ -592,6 +601,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -844,7 +856,7 @@
       </c>
       <c r="M18" s="15" t="str">
         <f t="shared" ref="M18:M19" si="1">K18/I18</f>
-        <v>0.87%</v>
+        <v>0.85%</v>
       </c>
     </row>
     <row r="19">
@@ -896,7 +908,7 @@
       </c>
       <c r="I21" s="14" t="str">
         <f>I51</f>
-        <v>718.23</v>
+        <v>717.00</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>27</v>
@@ -1087,7 +1099,7 @@
         <f>E38/C38</f>
         <v>1.00%</v>
       </c>
-      <c r="I38" s="22">
+      <c r="I38" s="28">
         <v>10.01</v>
       </c>
       <c r="J38" s="1" t="s">
@@ -1121,9 +1133,9 @@
       <c r="D39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="30"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="31"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
@@ -1156,7 +1168,7 @@
       <c r="J40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K40" s="31" t="str">
+      <c r="K40" s="32" t="str">
         <f>7*0.03</f>
         <v>0.21</v>
       </c>
@@ -1198,7 +1210,7 @@
         <f>E42/C42</f>
         <v>2.24%</v>
       </c>
-      <c r="H42" s="32"/>
+      <c r="H42" s="33"/>
       <c r="I42" s="14" t="str">
         <f>I38/(I40*C31)*10^6*C30</f>
         <v>1,500.12</v>
@@ -1223,21 +1235,21 @@
       <c r="A43" s="7"/>
     </row>
     <row r="44">
-      <c r="A44" s="33" t="s">
+      <c r="A44" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
-      <c r="K44" s="34"/>
-      <c r="L44" s="34"/>
-      <c r="M44" s="34"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="35"/>
     </row>
     <row r="46">
       <c r="A46" s="7"/>
@@ -1264,11 +1276,11 @@
       <c r="A47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C47" s="35" t="str">
+      <c r="C47" s="36" t="str">
         <f>C51/I42</f>
         <v>0.479</v>
       </c>
-      <c r="E47" s="35" t="str">
+      <c r="E47" s="36" t="str">
         <f>sqrt((1/(C48+C49)^4)*(C48^2*E49^2+C49^2*E48^2))</f>
         <v>0.004</v>
       </c>
@@ -1276,11 +1288,11 @@
         <f t="shared" ref="G47:G51" si="2">E47/C47</f>
         <v>0.74%</v>
       </c>
-      <c r="I47" s="36" t="str">
+      <c r="I47" s="37" t="str">
         <f>I48/I50</f>
         <v>0.47878</v>
       </c>
-      <c r="K47" s="36" t="str">
+      <c r="K47" s="37" t="str">
         <f>sqrt((1/(I50^4))*(I48^2*K49^2+I49^2*K48^2))</f>
         <v>0.00094</v>
       </c>
@@ -1293,7 +1305,7 @@
       <c r="A48" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C48" s="35" t="str">
+      <c r="C48" s="36" t="str">
         <f>C50*C51/I42</f>
         <v>4.309</v>
       </c>
@@ -1335,7 +1347,7 @@
       <c r="A49" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C49" s="35" t="str">
+      <c r="C49" s="36" t="str">
         <f>C50-C48</f>
         <v>4.691</v>
       </c>
@@ -1404,21 +1416,24 @@
       <c r="J50" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K50" s="35" t="str">
-        <f>sqrt(K48^2+K49^2)</f>
-        <v>0.017</v>
+      <c r="K50" s="36" t="str">
+        <f>K48+K49</f>
+        <v>0.024</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>16</v>
       </c>
       <c r="M50" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>0.19%</v>
+        <v>0.27%</v>
+      </c>
+      <c r="N50" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C51" s="14" t="str">
         <f>C21</f>
@@ -1427,7 +1442,7 @@
       <c r="D51" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E51" s="37" t="str">
+      <c r="E51" s="38" t="str">
         <f>sqrt(C47^2*E42^2+C42^2*E47^2)</f>
         <v>17</v>
       </c>
@@ -1438,14 +1453,13 @@
         <f t="shared" si="2"/>
         <v>2.35%</v>
       </c>
-      <c r="I51" s="37" t="str">
-        <f>I47*I42</f>
-        <v>718</v>
+      <c r="I51" s="39">
+        <v>717.0</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K51" s="37" t="str">
+      <c r="K51" s="38" t="str">
         <f>sqrt(I47^2*K42^2+I42^2*K47^2)</f>
         <v>9</v>
       </c>
@@ -1457,62 +1471,62 @@
         <v>1.21%</v>
       </c>
       <c r="N51" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B53" s="39"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="39"/>
-      <c r="J53" s="39"/>
-      <c r="K53" s="39"/>
-      <c r="L53" s="39"/>
-      <c r="M53" s="39"/>
+      <c r="A53" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="41"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="41"/>
+      <c r="J53" s="41"/>
+      <c r="K53" s="41"/>
+      <c r="L53" s="41"/>
+      <c r="M53" s="41"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B57" s="40"/>
+      <c r="B57" s="42"/>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="s">
-        <v>80</v>
+      <c r="A58" s="43" t="s">
+        <v>81</v>
       </c>
       <c r="C58" s="8">
         <v>50070.0</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C59" s="24">
         <v>1.0</v>
@@ -1522,8 +1536,8 @@
       <c r="A60" s="7"/>
     </row>
     <row r="61">
-      <c r="A61" s="41" t="s">
-        <v>83</v>
+      <c r="A61" s="44" t="s">
+        <v>84</v>
       </c>
       <c r="B61" s="26"/>
       <c r="C61" s="26"/>
@@ -1536,50 +1550,50 @@
       <c r="J61" s="26"/>
       <c r="K61" s="26"/>
       <c r="L61" s="26"/>
-      <c r="M61" s="42"/>
-      <c r="N61" s="43"/>
+      <c r="M61" s="45"/>
+      <c r="N61" s="46"/>
     </row>
     <row r="62">
-      <c r="A62" s="44"/>
+      <c r="A62" s="47"/>
       <c r="I62" s="12" t="s">
         <v>23</v>
       </c>
       <c r="K62" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="M62" s="45"/>
-      <c r="N62" s="44"/>
+      <c r="M62" s="48"/>
+      <c r="N62" s="47"/>
     </row>
     <row r="63">
-      <c r="A63" s="46" t="s">
-        <v>84</v>
+      <c r="A63" s="49" t="s">
+        <v>85</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I63" s="22">
         <v>11.768</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K63" s="22">
-        <v>0.03</v>
+        <v>87</v>
+      </c>
+      <c r="K63" s="28">
+        <v>0.02</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M63" s="15" t="str">
         <f t="shared" ref="M63:M65" si="5">K63/I63</f>
-        <v>0.25%</v>
+        <v>0.17%</v>
       </c>
       <c r="N63" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="46" t="s">
-        <v>88</v>
+      <c r="A64" s="49" t="s">
+        <v>89</v>
       </c>
       <c r="I64" s="14" t="str">
         <f>I63/C58*1000000</f>
@@ -1590,19 +1604,19 @@
       </c>
       <c r="K64" s="14" t="str">
         <f>I64*(K63/I63)</f>
-        <v>0.60</v>
+        <v>0.40</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>27</v>
       </c>
       <c r="M64" s="15" t="str">
         <f t="shared" si="5"/>
-        <v>0.25%</v>
+        <v>0.17%</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="46" t="s">
-        <v>89</v>
+      <c r="A65" s="49" t="s">
+        <v>90</v>
       </c>
       <c r="I65" s="14" t="str">
         <f>C59*I64</f>
@@ -1613,24 +1627,24 @@
       </c>
       <c r="K65" s="14" t="str">
         <f>C59*K64</f>
-        <v>0.60</v>
+        <v>0.40</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>27</v>
       </c>
       <c r="M65" s="15" t="str">
         <f t="shared" si="5"/>
-        <v>0.25%</v>
+        <v>0.17%</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="43"/>
-      <c r="M66" s="45"/>
-      <c r="N66" s="43"/>
+      <c r="A66" s="46"/>
+      <c r="M66" s="48"/>
+      <c r="N66" s="46"/>
     </row>
     <row r="67">
-      <c r="A67" s="41" t="s">
-        <v>90</v>
+      <c r="A67" s="44" t="s">
+        <v>91</v>
       </c>
       <c r="B67" s="26"/>
       <c r="C67" s="26"/>
@@ -1643,13 +1657,13 @@
       <c r="J67" s="26"/>
       <c r="K67" s="26"/>
       <c r="L67" s="26"/>
-      <c r="M67" s="42"/>
-      <c r="N67" s="46" t="s">
-        <v>91</v>
+      <c r="M67" s="45"/>
+      <c r="N67" s="49" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="43"/>
+      <c r="A68" s="46"/>
       <c r="C68" s="12" t="s">
         <v>22</v>
       </c>
@@ -1668,21 +1682,21 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C69" s="36" t="str">
+        <v>93</v>
+      </c>
+      <c r="C69" s="37" t="str">
         <f>C73/I65</f>
         <v>0.04255</v>
       </c>
-      <c r="E69" s="36" t="str">
+      <c r="E69" s="37" t="str">
         <f>sqrt((1/(C70+C71)^4)*(C70^2*E71^2+C71^2*E70^2))</f>
         <v>0.00058</v>
       </c>
-      <c r="I69" s="36" t="str">
+      <c r="I69" s="37" t="str">
         <f>I70/I72</f>
         <v>0.04258</v>
       </c>
-      <c r="K69" s="36" t="str">
+      <c r="K69" s="37" t="str">
         <f>I69*(1-I69)*sqrt((K70/I70)^2+(K71/I71)^2)</f>
         <v>0.00036</v>
       </c>
@@ -1695,21 +1709,21 @@
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C70" s="35" t="str">
+      <c r="C70" s="36" t="str">
         <f>C72*C73/I65</f>
         <v>0.511</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="35" t="str">
+      <c r="E70" s="36" t="str">
         <f t="shared" ref="E70:E71" si="7">0.01*C70</f>
         <v>0.005</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I70" s="47">
+      <c r="I70" s="50">
         <v>0.511</v>
       </c>
       <c r="J70" s="1" t="s">
@@ -1726,14 +1740,14 @@
         <v>0.78%</v>
       </c>
       <c r="N70" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="35" t="str">
+      <c r="C71" s="36" t="str">
         <f>C72-C70</f>
         <v>11.489</v>
       </c>
@@ -1747,13 +1761,13 @@
       <c r="F71" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I71" s="47">
+      <c r="I71" s="50">
         <v>11.489</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K71" s="48" t="str">
+      <c r="K71" s="51" t="str">
         <f>sqrt(0.03^2 + 0.03^2 + 0.012^2)</f>
         <v>0.044</v>
       </c>
@@ -1765,15 +1779,15 @@
         <v>0.38%</v>
       </c>
       <c r="N71" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C72" s="13">
         <v>12.0</v>
@@ -1795,7 +1809,7 @@
       <c r="J72" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K72" s="35" t="str">
+      <c r="K72" s="36" t="str">
         <f>sqrt(K70^2+K71^2)</f>
         <v>0.044</v>
       </c>
@@ -1809,7 +1823,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C73" s="14" t="str">
         <f>C18</f>
@@ -1832,48 +1846,48 @@
       <c r="J73" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K73" s="35" t="str">
+      <c r="K73" s="36" t="str">
         <f>sqrt(I69^2*K65^2+I65^2*K69^2)</f>
-        <v>0.087</v>
+        <v>0.085</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>27</v>
       </c>
       <c r="M73" s="15" t="str">
         <f t="shared" si="6"/>
-        <v>0.87%</v>
+        <v>0.85%</v>
       </c>
       <c r="N73" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="B75" s="50"/>
-      <c r="C75" s="50"/>
-      <c r="D75" s="50"/>
-      <c r="E75" s="50"/>
-      <c r="F75" s="50"/>
-      <c r="G75" s="50"/>
-      <c r="H75" s="50"/>
-      <c r="I75" s="50"/>
-      <c r="J75" s="50"/>
-      <c r="K75" s="50"/>
-      <c r="L75" s="50"/>
-      <c r="M75" s="50"/>
-      <c r="N75" s="50"/>
+      <c r="A75" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B75" s="53"/>
+      <c r="C75" s="53"/>
+      <c r="D75" s="53"/>
+      <c r="E75" s="53"/>
+      <c r="F75" s="53"/>
+      <c r="G75" s="53"/>
+      <c r="H75" s="53"/>
+      <c r="I75" s="53"/>
+      <c r="J75" s="53"/>
+      <c r="K75" s="53"/>
+      <c r="L75" s="53"/>
+      <c r="M75" s="53"/>
+      <c r="N75" s="53"/>
     </row>
     <row r="77">
       <c r="C77" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G77" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I77" s="12" t="s">
         <v>23</v>
@@ -1887,12 +1901,12 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C78" s="22">
         <v>0.915</v>
       </c>
-      <c r="E78" s="47">
+      <c r="E78" s="50">
         <v>0.00339</v>
       </c>
       <c r="G78" s="15" t="str">
@@ -1903,51 +1917,51 @@
         <f t="shared" ref="I78:I79" si="9">C78</f>
         <v>0.915</v>
       </c>
-      <c r="K78" s="35" t="str">
+      <c r="K78" s="36" t="str">
         <f t="shared" ref="K78:K79" si="10">C78*sqrt((E78/C78)^2 + (K50/I50)^2)</f>
         <v>0.004</v>
       </c>
       <c r="M78" s="15" t="str">
         <f t="shared" ref="M78:M80" si="11">K78/I78</f>
-        <v>0.42%</v>
+        <v>0.46%</v>
       </c>
       <c r="N78" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C79" s="51">
+        <v>106</v>
+      </c>
+      <c r="C79" s="54">
         <v>1200000.0</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E79" s="51">
+        <v>107</v>
+      </c>
+      <c r="E79" s="54">
         <v>27800.0</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G79" s="15" t="str">
         <f t="shared" si="8"/>
         <v>2.32%</v>
       </c>
-      <c r="I79" s="52" t="str">
+      <c r="I79" s="55" t="str">
         <f t="shared" si="9"/>
         <v>1.20E+06</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K79" s="52" t="str">
+        <v>107</v>
+      </c>
+      <c r="K79" s="55" t="str">
         <f t="shared" si="10"/>
         <v>3.14E+04</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M79" s="15" t="str">
         <f t="shared" si="11"/>
@@ -1956,39 +1970,39 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C80" s="52" t="str">
+        <v>108</v>
+      </c>
+      <c r="C80" s="55" t="str">
         <f>1/C79</f>
         <v>8.33E-07</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E80" s="52" t="str">
+        <v>109</v>
+      </c>
+      <c r="E80" s="55" t="str">
         <f>E79/(C79^2)</f>
         <v>1.93E-08</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G80" s="15" t="str">
         <f t="shared" si="8"/>
         <v>2.32%</v>
       </c>
-      <c r="I80" s="52" t="str">
+      <c r="I80" s="55" t="str">
         <f>1/I79</f>
         <v>8.33E-07</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K80" s="52" t="str">
+        <v>109</v>
+      </c>
+      <c r="K80" s="55" t="str">
         <f>K79/(I79^2)</f>
         <v>2.18E-08</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M80" s="15" t="str">
         <f t="shared" si="11"/>
@@ -1997,19 +2011,19 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C81" s="22">
         <v>-11.27</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E81" s="22">
         <v>0.05721</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G81" s="15" t="str">
         <f t="shared" ref="G81:G83" si="12">abs(E81/C81)</f>
@@ -2020,14 +2034,14 @@
         <v>-11.27</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K81" s="14" t="str">
         <f>abs(C81)*sqrt((E81/C81)^2+(K51/I51)^2)</f>
         <v>0.15</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M81" s="15" t="str">
         <f t="shared" ref="M81:M83" si="13">abs(K81/I81)</f>
@@ -2036,21 +2050,21 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C82" s="14" t="str">
         <f>C81-C83</f>
         <v>-2.97</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E82" s="14" t="str">
         <f>sqrt(E83^2+E81^2)</f>
         <v>0.06</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G82" s="15" t="str">
         <f t="shared" si="12"/>
@@ -2061,14 +2075,14 @@
         <v>-2.97</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K82" s="14" t="str">
         <f>sqrt(K83^2+K81^2)</f>
         <v>0.15</v>
       </c>
       <c r="L82" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M82" s="15" t="str">
         <f t="shared" si="13"/>
@@ -2077,21 +2091,21 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C83" s="14" t="str">
         <f>-1.381*6.022/4184*(273.15+C9)*ln(C79)</f>
         <v>-8.30</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E83" s="14" t="str">
         <f>1.381*6.022/4184*(273.15+C9)*(E79/C79)</f>
         <v>0.01</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G83" s="15" t="str">
         <f t="shared" si="12"/>
@@ -2102,14 +2116,14 @@
         <v>-8.30</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K83" s="14" t="str">
         <f>1.381*6.022/4184*(273.15+C9)*(K79/I79)</f>
         <v>0.02</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M83" s="15" t="str">
         <f t="shared" si="13"/>

</xml_diff>